<commit_message>
taken API useage out of main call in modeselector, added prcipitation data for rain effect
</commit_message>
<xml_diff>
--- a/Inputs/Yaz_Journey_API_inputs_data.xlsx
+++ b/Inputs/Yaz_Journey_API_inputs_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/DP5_new_mod/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{219950F0-FE0A-2D4E-9FFB-2D6A8BA94DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669DB5D1-B051-4940-8306-AC8FAB1B1082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="1100" windowWidth="28920" windowHeight="18600" xr2:uid="{7BA55488-F6DA-4B4E-A73F-1D457F286A83}"/>
+    <workbookView xWindow="6920" yWindow="1040" windowWidth="28920" windowHeight="18600" xr2:uid="{7BA55488-F6DA-4B4E-A73F-1D457F286A83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Number</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Cost of Change</t>
   </si>
   <si>
-    <t>Battery Properties</t>
-  </si>
-  <si>
     <t>Battery Capacity</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Heating</t>
   </si>
   <si>
-    <t xml:space="preserve">Cooling </t>
-  </si>
-  <si>
     <t>Driving Style</t>
   </si>
   <si>
@@ -126,13 +120,22 @@
     <t>Current Household of 4</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Bristol, UK, BS8 2AB</t>
   </si>
   <si>
     <t>Bristol, UK, BS1 2NJ</t>
+  </si>
+  <si>
+    <t>Carbon Kg per litre Fuel</t>
+  </si>
+  <si>
+    <t>London, UK, HA5 5SG</t>
+  </si>
+  <si>
+    <t>Vehicle  Properties</t>
+  </si>
+  <si>
+    <t>Cooling</t>
   </si>
 </sst>
 </file>
@@ -221,15 +224,37 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -567,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2E5EC4-C63E-7541-9E04-A7322ACAA217}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,17 +606,17 @@
     <col min="4" max="4" width="3.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" customWidth="1"/>
-    <col min="15" max="15" width="3.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -600,7 +625,7 @@
     <col min="28" max="28" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="129" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="129" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,84 +642,87 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
+      <c r="AC1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7">
@@ -705,34 +733,34 @@
         <v>54</v>
       </c>
       <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <v>355</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1684</v>
+      </c>
+      <c r="K2" s="7">
         <v>7.4</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10">
-        <v>43522.291666666664</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="10">
+        <v>44253.291666666664</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="10">
-        <v>43522.305555555555</v>
-      </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>355</v>
-      </c>
-      <c r="R2" s="7">
-        <v>1684</v>
-      </c>
+      <c r="Q2" s="10">
+        <v>44253.305555555555</v>
+      </c>
+      <c r="R2" s="9"/>
       <c r="S2" s="7">
         <v>1</v>
       </c>
@@ -763,21 +791,39 @@
       <c r="AB2" s="7">
         <v>50</v>
       </c>
+      <c r="AC2">
+        <v>2.31</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AA2:XFD2 A2:J2 N2:O2">
-    <cfRule type="expression" dxfId="2" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="AA2:AB2 A2:M2 Q2:R2 AD2:XFD2">
+    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
       <formula>A2&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="M2">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="lessThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>M2</formula>
+  <conditionalFormatting sqref="Q2">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>P2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>AC2&lt;&gt;AC1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:P2">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>N2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:P2">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>O2&lt;&gt;O1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>